<commit_message>
Added descriptors for dermal and aerosol routes
</commit_message>
<xml_diff>
--- a/CvT_data_template_articles.xlsx
+++ b/CvT_data_template_articles.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CGrulke\IdeaProjects\CompTox-PK-CvTdb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85469376-95F4-493A-86BE-D770A80D4B32}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84C6092-CD81-4333-A597-AF1252274A24}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>id</t>
   </si>
@@ -153,6 +153,33 @@
   </si>
   <si>
     <t>fk_series_id</t>
+  </si>
+  <si>
+    <t>aerosol_particle_diameter_mean</t>
+  </si>
+  <si>
+    <t>aerosol_particle_diameter_gsd</t>
+  </si>
+  <si>
+    <t>aerosol_particle_density</t>
+  </si>
+  <si>
+    <t>aerosol_particle_diameter_units</t>
+  </si>
+  <si>
+    <t>aerosol_particle_density_units</t>
+  </si>
+  <si>
+    <t>dermal_applied_area</t>
+  </si>
+  <si>
+    <t>dermal_applied_area_units</t>
+  </si>
+  <si>
+    <t>dermal_dose_vehicle</t>
+  </si>
+  <si>
+    <t>dermal_dose_vehicle_pH</t>
   </si>
 </sst>
 </file>
@@ -518,7 +545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99E831F9-6B15-4914-9CE1-426B4CF01319}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -560,10 +587,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBCE4BB7-D604-4848-8F98-B3DF84410C96}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,7 +609,7 @@
     <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -618,6 +645,33 @@
       </c>
       <c r="L1" s="8" t="s">
         <v>35</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -17317,7 +17371,7 @@
   <dimension ref="A1:R399"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>